<commit_message>
#26 Gantt chart frissitése - feltöltés a szükséges adatokkal
</commit_message>
<xml_diff>
--- a/dokumentumok/Gantt_chart_excel_sablon.xlsx
+++ b/dokumentumok/Gantt_chart_excel_sablon.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>Projekttervező</t>
   </si>
@@ -182,9 +182,6 @@
     <t>Kovács Tamás</t>
   </si>
   <si>
-    <t>Hamad Aszim</t>
-  </si>
-  <si>
     <t>Class diagram</t>
   </si>
   <si>
@@ -258,6 +255,19 @@
   </si>
   <si>
     <t>Tesztelési dokumentum az új funkciókhoz</t>
+  </si>
+  <si>
+    <t>Tesztdokumentumok áttekintése</t>
+  </si>
+  <si>
+    <t>Spring security áttekintése</t>
+  </si>
+  <si>
+    <t>Veres-Lakos Zsombor</t>
+  </si>
+  <si>
+    <t>design elképzelése
+Design elképzelése</t>
   </si>
 </sst>
 </file>
@@ -968,7 +978,7 @@
     <xf numFmtId="0" fontId="1" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1041,6 +1051,24 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1050,12 +1078,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1086,17 +1108,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1160,7 +1173,7 @@
     <cellStyle name="Terv jelmagyarázata" xfId="14"/>
     <cellStyle name="Tevékenység" xfId="2"/>
   </cellStyles>
-  <dxfs count="111">
+  <dxfs count="126">
     <dxf>
       <fill>
         <patternFill>
@@ -1390,34 +1403,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -1429,100 +1414,7 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1542,100 +1434,7 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1655,100 +1454,7 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1768,100 +1474,7 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1881,100 +1494,7 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
+          <color theme="7"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -1994,75 +1514,10 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
+          <color theme="7"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2407,6 +1862,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -2418,7 +1901,100 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -2438,7 +2014,100 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -2458,7 +2127,100 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -2478,7 +2240,100 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -2498,7 +2353,100 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -2518,7 +2466,100 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
         </bottom>
         <vertical/>
         <horizontal/>
@@ -2538,10 +2579,188 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3014,10 +3233,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:CG27"/>
+  <dimension ref="B1:CG30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AG6" sqref="AG6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AL16" sqref="AL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3045,79 +3264,79 @@
       <c r="G1" s="7"/>
     </row>
     <row r="2" spans="2:85" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="37"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="41"/>
+      <c r="U2" s="41"/>
+      <c r="V2" s="41"/>
       <c r="W2" s="10"/>
-      <c r="X2" s="34" t="s">
+      <c r="X2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
       <c r="AA2" s="11"/>
-      <c r="AB2" s="34" t="s">
+      <c r="AB2" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="35"/>
-      <c r="AH2" s="35"/>
-      <c r="AI2" s="35"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
       <c r="AJ2" s="12"/>
-      <c r="AK2" s="24" t="s">
+      <c r="AK2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
-      <c r="AR2" s="25"/>
+      <c r="AL2" s="31"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="31"/>
+      <c r="AO2" s="31"/>
+      <c r="AP2" s="31"/>
+      <c r="AQ2" s="31"/>
+      <c r="AR2" s="31"/>
     </row>
     <row r="3" spans="2:85" s="6" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -3136,12 +3355,12 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="2:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="H4" s="13">
         <v>44088</v>
       </c>
@@ -3378,7 +3597,7 @@
       </c>
     </row>
     <row r="5" spans="2:85" ht="70.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="14" t="s">
@@ -3420,7 +3639,7 @@
       <c r="AC5" s="11"/>
     </row>
     <row r="6" spans="2:85" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="40"/>
+      <c r="B6" s="27"/>
       <c r="C6" s="14" t="s">
         <v>21</v>
       </c>
@@ -3459,8 +3678,8 @@
       <c r="AB6" s="11"/>
       <c r="AC6" s="11"/>
     </row>
-    <row r="7" spans="2:85" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="41" t="s">
+    <row r="7" spans="2:85" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="28" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="21" t="s">
@@ -3470,13 +3689,13 @@
         <v>23</v>
       </c>
       <c r="E7" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F7" s="13">
         <v>44110</v>
       </c>
       <c r="G7" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
@@ -3500,7 +3719,7 @@
       <c r="AA7" s="20"/>
       <c r="AB7" s="18"/>
       <c r="AC7" s="18"/>
-      <c r="AD7" s="11"/>
+      <c r="AD7" s="18"/>
       <c r="AE7" s="18"/>
       <c r="AF7" s="18"/>
       <c r="AG7" s="18"/>
@@ -3557,16 +3776,16 @@
       <c r="CF7" s="18"/>
       <c r="CG7" s="18"/>
     </row>
-    <row r="8" spans="2:85" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="42"/>
+    <row r="8" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="29"/>
       <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="16">
-        <v>5</v>
+        <v>51</v>
+      </c>
+      <c r="E8" s="43">
+        <v>1</v>
       </c>
       <c r="F8" s="13">
         <v>44110</v>
@@ -3574,52 +3793,65 @@
       <c r="G8" s="4">
         <v>3</v>
       </c>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+      <c r="AL8" s="18"/>
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="18"/>
+      <c r="AO8" s="18"/>
+      <c r="AP8" s="18"/>
+      <c r="AQ8" s="18"/>
+      <c r="AR8" s="18"/>
     </row>
-    <row r="9" spans="2:85" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="42"/>
+    <row r="9" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="29"/>
       <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="16">
-        <v>6</v>
+      <c r="E9" s="43">
+        <v>3</v>
       </c>
       <c r="F9" s="13">
         <v>44114</v>
       </c>
       <c r="G9" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AD9" s="18"/>
       <c r="AE9" s="18"/>
       <c r="AF9" s="18"/>
       <c r="AG9" s="18"/>
-      <c r="AH9" s="11"/>
-      <c r="AI9" s="11"/>
-      <c r="AJ9" s="11"/>
-      <c r="AK9" s="11"/>
-      <c r="AL9" s="11"/>
-      <c r="AM9" s="11"/>
-      <c r="AN9" s="11"/>
-      <c r="AO9" s="11"/>
-      <c r="AP9" s="11"/>
-      <c r="AQ9" s="11"/>
+      <c r="AH9" s="18"/>
+      <c r="AI9" s="18"/>
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="18"/>
+      <c r="AM9" s="18"/>
+      <c r="AN9" s="18"/>
+      <c r="AO9" s="18"/>
+      <c r="AP9" s="18"/>
+      <c r="AQ9" s="18"/>
+      <c r="AR9" s="18"/>
     </row>
-    <row r="10" spans="2:85" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="42"/>
+    <row r="10" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="29"/>
       <c r="C10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="16">
-        <v>5</v>
+      <c r="E10" s="43">
+        <v>2</v>
       </c>
       <c r="F10" s="13">
         <v>44110</v>
@@ -3627,21 +3859,32 @@
       <c r="G10" s="4">
         <v>3</v>
       </c>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
-      <c r="AG10" s="11"/>
+      <c r="AD10" s="18"/>
+      <c r="AE10" s="18"/>
+      <c r="AF10" s="18"/>
+      <c r="AG10" s="18"/>
+      <c r="AH10" s="18"/>
+      <c r="AI10" s="18"/>
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+      <c r="AL10" s="18"/>
+      <c r="AM10" s="18"/>
+      <c r="AN10" s="18"/>
+      <c r="AO10" s="18"/>
+      <c r="AP10" s="18"/>
+      <c r="AQ10" s="18"/>
+      <c r="AR10" s="18"/>
     </row>
-    <row r="11" spans="2:85" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="42"/>
+    <row r="11" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="29"/>
       <c r="C11" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="16">
-        <v>5</v>
+        <v>20</v>
+      </c>
+      <c r="E11" s="43">
+        <v>2</v>
       </c>
       <c r="F11" s="13">
         <v>44111</v>
@@ -3649,130 +3892,138 @@
       <c r="G11" s="4">
         <v>3</v>
       </c>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
+      <c r="AD11" s="18"/>
+      <c r="AE11" s="18"/>
+      <c r="AF11" s="18"/>
+      <c r="AG11" s="18"/>
+      <c r="AH11" s="18"/>
+      <c r="AI11" s="18"/>
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+      <c r="AL11" s="18"/>
+      <c r="AM11" s="18"/>
+      <c r="AN11" s="18"/>
+      <c r="AO11" s="18"/>
+      <c r="AP11" s="18"/>
+      <c r="AQ11" s="18"/>
+      <c r="AR11" s="18"/>
     </row>
-    <row r="12" spans="2:85" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="42"/>
+    <row r="12" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="29"/>
       <c r="C12" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="16">
-        <v>5</v>
+      <c r="E12" s="43">
+        <v>3</v>
       </c>
       <c r="F12" s="13">
-        <v>44112</v>
+        <v>44119</v>
       </c>
       <c r="G12" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="AD12" s="18"/>
       <c r="AE12" s="18"/>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="11"/>
-      <c r="AI12" s="11"/>
-      <c r="AJ12" s="11"/>
-      <c r="AK12" s="11"/>
-      <c r="AL12" s="11"/>
-      <c r="AM12" s="11"/>
-      <c r="AN12" s="11"/>
+      <c r="AF12" s="18"/>
+      <c r="AG12" s="18"/>
+      <c r="AH12" s="18"/>
+      <c r="AI12" s="18"/>
+      <c r="AJ12" s="18"/>
+      <c r="AK12" s="18"/>
+      <c r="AL12" s="18"/>
+      <c r="AM12" s="18"/>
+      <c r="AN12" s="18"/>
       <c r="AO12" s="18"/>
       <c r="AP12" s="18"/>
       <c r="AQ12" s="18"/>
+      <c r="AR12" s="18"/>
     </row>
-    <row r="13" spans="2:85" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="42"/>
+    <row r="13" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="29"/>
       <c r="C13" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="43">
+        <v>3</v>
+      </c>
+      <c r="F13" s="13">
+        <v>44112</v>
+      </c>
+      <c r="G13" s="4">
+        <v>5</v>
+      </c>
+      <c r="AD13" s="18"/>
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="18"/>
+      <c r="AG13" s="18"/>
+      <c r="AH13" s="18"/>
+      <c r="AI13" s="18"/>
+      <c r="AJ13" s="18"/>
+      <c r="AK13" s="18"/>
+      <c r="AL13" s="18"/>
+      <c r="AM13" s="18"/>
+      <c r="AN13" s="18"/>
+      <c r="AO13" s="18"/>
+      <c r="AP13" s="18"/>
+      <c r="AQ13" s="18"/>
+      <c r="AR13" s="18"/>
+    </row>
+    <row r="14" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="29"/>
+      <c r="C14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E14" s="43">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13">
+        <v>44124</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3</v>
+      </c>
+      <c r="AD14" s="18"/>
+      <c r="AE14" s="18"/>
+      <c r="AF14" s="18"/>
+      <c r="AG14" s="18"/>
+      <c r="AH14" s="18"/>
+      <c r="AI14" s="18"/>
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+      <c r="AL14" s="18"/>
+      <c r="AM14" s="18"/>
+      <c r="AN14" s="18"/>
+      <c r="AO14" s="18"/>
+      <c r="AP14" s="18"/>
+      <c r="AQ14" s="18"/>
+      <c r="AR14" s="18"/>
+    </row>
+    <row r="15" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="29"/>
+      <c r="C15" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="43">
+        <v>2</v>
+      </c>
+      <c r="F15" s="13">
+        <v>44119</v>
+      </c>
+      <c r="G15" s="4">
         <v>5</v>
       </c>
-      <c r="F13" s="13">
-        <v>44110</v>
-      </c>
-      <c r="G13" s="4">
-        <v>3</v>
-      </c>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11"/>
-    </row>
-    <row r="14" spans="2:85" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="40"/>
-      <c r="C14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="16">
-        <v>5</v>
-      </c>
-      <c r="F14" s="13">
-        <v>44111</v>
-      </c>
-      <c r="G14" s="4">
-        <v>6</v>
-      </c>
-      <c r="AD14" s="18"/>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11"/>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11"/>
-    </row>
-    <row r="15" spans="2:85" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="22">
-        <v>4</v>
-      </c>
-      <c r="F15" s="17">
-        <v>44124</v>
-      </c>
-      <c r="G15" s="19">
-        <v>8</v>
-      </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="20"/>
-      <c r="V15" s="20"/>
-      <c r="W15" s="20"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="20"/>
-      <c r="Z15" s="20"/>
-      <c r="AA15" s="20"/>
-      <c r="AB15" s="18"/>
-      <c r="AC15" s="18"/>
       <c r="AD15" s="18"/>
       <c r="AE15" s="18"/>
       <c r="AF15" s="18"/>
@@ -3788,351 +4039,469 @@
       <c r="AP15" s="18"/>
       <c r="AQ15" s="18"/>
       <c r="AR15" s="18"/>
-      <c r="AS15" s="18"/>
-      <c r="AT15" s="18"/>
-      <c r="AU15" s="18"/>
-      <c r="AV15" s="18"/>
-      <c r="AW15" s="18"/>
-      <c r="AX15" s="18"/>
-      <c r="AY15" s="18"/>
-      <c r="AZ15" s="18"/>
-      <c r="BA15" s="18"/>
-      <c r="BB15" s="18"/>
-      <c r="BC15" s="18"/>
-      <c r="BD15" s="18"/>
-      <c r="BE15" s="18"/>
-      <c r="BF15" s="18"/>
-      <c r="BG15" s="18"/>
-      <c r="BH15" s="18"/>
-      <c r="BI15" s="18"/>
-      <c r="BJ15" s="18"/>
-      <c r="BK15" s="18"/>
-      <c r="BL15" s="18"/>
-      <c r="BM15" s="18"/>
-      <c r="BN15" s="18"/>
-      <c r="BO15" s="18"/>
-      <c r="BP15" s="18"/>
-      <c r="BQ15" s="18"/>
-      <c r="BR15" s="18"/>
-      <c r="BS15" s="18"/>
-      <c r="BT15" s="18"/>
-      <c r="BU15" s="18"/>
-      <c r="BV15" s="18"/>
-      <c r="BW15" s="18"/>
-      <c r="BX15" s="18"/>
-      <c r="BY15" s="18"/>
-      <c r="BZ15" s="18"/>
-      <c r="CA15" s="18"/>
-      <c r="CB15" s="18"/>
-      <c r="CC15" s="18"/>
-      <c r="CD15" s="18"/>
-      <c r="CE15" s="18"/>
-      <c r="CF15" s="18"/>
-      <c r="CG15" s="18"/>
     </row>
     <row r="16" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="42"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="14" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="16">
-        <v>10</v>
-      </c>
-      <c r="F16" s="17">
-        <v>44124</v>
+        <v>42</v>
+      </c>
+      <c r="E16" s="43">
+        <v>3</v>
+      </c>
+      <c r="F16" s="13">
+        <v>44123</v>
       </c>
       <c r="G16" s="4">
-        <v>10</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="18"/>
+      <c r="AI16" s="18"/>
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="18"/>
+      <c r="AL16" s="18"/>
+      <c r="AM16" s="18"/>
+      <c r="AN16" s="18"/>
+      <c r="AO16" s="18"/>
+      <c r="AP16" s="18"/>
+      <c r="AQ16" s="18"/>
+      <c r="AR16" s="18"/>
     </row>
     <row r="17" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="42"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>40</v>
+        <v>26</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="E17" s="16">
-        <v>5</v>
-      </c>
-      <c r="F17" s="17">
-        <v>44125</v>
+        <v>3</v>
+      </c>
+      <c r="F17" s="13">
+        <v>44111</v>
       </c>
       <c r="G17" s="4">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="AD17" s="18"/>
+      <c r="AE17" s="18"/>
+      <c r="AF17" s="18"/>
+      <c r="AG17" s="18"/>
+      <c r="AH17" s="18"/>
+      <c r="AI17" s="18"/>
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+      <c r="AL17" s="18"/>
+      <c r="AM17" s="18"/>
+      <c r="AN17" s="18"/>
+      <c r="AO17" s="18"/>
+      <c r="AP17" s="18"/>
+      <c r="AQ17" s="18"/>
+      <c r="AR17" s="18"/>
     </row>
     <row r="18" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="42"/>
-      <c r="C18" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="16">
-        <v>5</v>
+      <c r="B18" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="22">
+        <v>4</v>
       </c>
       <c r="F18" s="17">
-        <v>44125</v>
-      </c>
-      <c r="G18" s="4">
-        <v>5</v>
-      </c>
+        <v>44124</v>
+      </c>
+      <c r="G18" s="19">
+        <v>8</v>
+      </c>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="20"/>
+      <c r="Q18" s="20"/>
+      <c r="R18" s="20"/>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="20"/>
+      <c r="W18" s="20"/>
+      <c r="X18" s="20"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="18"/>
+      <c r="AC18" s="18"/>
+      <c r="AD18" s="18"/>
+      <c r="AE18" s="18"/>
+      <c r="AF18" s="18"/>
+      <c r="AG18" s="18"/>
+      <c r="AH18" s="18"/>
+      <c r="AI18" s="18"/>
+      <c r="AJ18" s="18"/>
+      <c r="AK18" s="18"/>
+      <c r="AL18" s="18"/>
+      <c r="AM18" s="18"/>
+      <c r="AN18" s="18"/>
+      <c r="AO18" s="18"/>
+      <c r="AP18" s="18"/>
+      <c r="AQ18" s="18"/>
+      <c r="AR18" s="18"/>
+      <c r="AS18" s="18"/>
+      <c r="AT18" s="18"/>
+      <c r="AU18" s="18"/>
+      <c r="AV18" s="18"/>
+      <c r="AW18" s="18"/>
+      <c r="AX18" s="18"/>
+      <c r="AY18" s="18"/>
+      <c r="AZ18" s="18"/>
+      <c r="BA18" s="18"/>
+      <c r="BB18" s="18"/>
+      <c r="BC18" s="18"/>
+      <c r="BD18" s="18"/>
+      <c r="BE18" s="18"/>
+      <c r="BF18" s="18"/>
+      <c r="BG18" s="18"/>
+      <c r="BH18" s="18"/>
+      <c r="BI18" s="18"/>
+      <c r="BJ18" s="18"/>
+      <c r="BK18" s="18"/>
+      <c r="BL18" s="18"/>
+      <c r="BM18" s="18"/>
+      <c r="BN18" s="18"/>
+      <c r="BO18" s="18"/>
+      <c r="BP18" s="18"/>
+      <c r="BQ18" s="18"/>
+      <c r="BR18" s="18"/>
+      <c r="BS18" s="18"/>
+      <c r="BT18" s="18"/>
+      <c r="BU18" s="18"/>
+      <c r="BV18" s="18"/>
+      <c r="BW18" s="18"/>
+      <c r="BX18" s="18"/>
+      <c r="BY18" s="18"/>
+      <c r="BZ18" s="18"/>
+      <c r="CA18" s="18"/>
+      <c r="CB18" s="18"/>
+      <c r="CC18" s="18"/>
+      <c r="CD18" s="18"/>
+      <c r="CE18" s="18"/>
+      <c r="CF18" s="18"/>
+      <c r="CG18" s="18"/>
     </row>
     <row r="19" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="42"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="14" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E19" s="16">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F19" s="17">
-        <v>44126</v>
+        <v>44124</v>
       </c>
       <c r="G19" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="42"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E20" s="16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" s="17">
-        <v>44127</v>
+        <v>44125</v>
       </c>
       <c r="G20" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="42"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="14" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E21" s="16">
         <v>5</v>
       </c>
       <c r="F21" s="17">
-        <v>44128</v>
+        <v>44125</v>
       </c>
       <c r="G21" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="42"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="14" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E22" s="16">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F22" s="17">
-        <v>44129</v>
+        <v>44126</v>
       </c>
       <c r="G22" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="22">
+      <c r="B23" s="29"/>
+      <c r="C23" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="16">
         <v>6</v>
       </c>
       <c r="F23" s="17">
-        <v>44138</v>
-      </c>
-      <c r="G23" s="19">
-        <v>3</v>
-      </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
-      <c r="T23" s="20"/>
-      <c r="U23" s="20"/>
-      <c r="V23" s="20"/>
-      <c r="W23" s="20"/>
-      <c r="X23" s="20"/>
-      <c r="Y23" s="20"/>
-      <c r="Z23" s="20"/>
-      <c r="AA23" s="20"/>
-      <c r="AB23" s="18"/>
-      <c r="AC23" s="18"/>
-      <c r="AD23" s="18"/>
-      <c r="AE23" s="18"/>
-      <c r="AF23" s="18"/>
-      <c r="AG23" s="18"/>
-      <c r="AH23" s="18"/>
-      <c r="AI23" s="18"/>
-      <c r="AJ23" s="18"/>
-      <c r="AK23" s="18"/>
-      <c r="AL23" s="18"/>
-      <c r="AM23" s="18"/>
-      <c r="AN23" s="18"/>
-      <c r="AO23" s="18"/>
-      <c r="AP23" s="18"/>
-      <c r="AQ23" s="18"/>
-      <c r="AR23" s="18"/>
-      <c r="AS23" s="18"/>
-      <c r="AT23" s="18"/>
-      <c r="AU23" s="18"/>
-      <c r="AV23" s="18"/>
-      <c r="AW23" s="18"/>
-      <c r="AX23" s="18"/>
-      <c r="AY23" s="18"/>
-      <c r="AZ23" s="18"/>
-      <c r="BA23" s="18"/>
-      <c r="BB23" s="18"/>
-      <c r="BC23" s="18"/>
-      <c r="BD23" s="18"/>
-      <c r="BE23" s="18"/>
-      <c r="BF23" s="18"/>
-      <c r="BG23" s="18"/>
-      <c r="BH23" s="18"/>
-      <c r="BI23" s="18"/>
-      <c r="BJ23" s="18"/>
-      <c r="BK23" s="18"/>
-      <c r="BL23" s="18"/>
-      <c r="BM23" s="18"/>
-      <c r="BN23" s="18"/>
-      <c r="BO23" s="18"/>
-      <c r="BP23" s="18"/>
-      <c r="BQ23" s="18"/>
-      <c r="BR23" s="18"/>
-      <c r="BS23" s="18"/>
-      <c r="BT23" s="18"/>
-      <c r="BU23" s="18"/>
-      <c r="BV23" s="18"/>
-      <c r="BW23" s="18"/>
-      <c r="BX23" s="18"/>
-      <c r="BY23" s="18"/>
-      <c r="BZ23" s="18"/>
-      <c r="CA23" s="18"/>
-      <c r="CB23" s="18"/>
-      <c r="CC23" s="18"/>
-      <c r="CD23" s="18"/>
-      <c r="CE23" s="18"/>
-      <c r="CF23" s="18"/>
-      <c r="CG23" s="18"/>
+        <v>44127</v>
+      </c>
+      <c r="G23" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="42"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="14" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E24" s="16">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F24" s="17">
-        <v>44139</v>
+        <v>44128</v>
       </c>
       <c r="G24" s="4">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="42"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="14" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E25" s="16">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F25" s="17">
-        <v>44140</v>
+        <v>44129</v>
       </c>
       <c r="G25" s="4">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="42"/>
-      <c r="C26" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="15" t="s">
+      <c r="B26" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="16">
-        <v>5</v>
+      <c r="E26" s="22">
+        <v>6</v>
       </c>
       <c r="F26" s="17">
-        <v>44141</v>
-      </c>
-      <c r="G26" s="4">
+        <v>44138</v>
+      </c>
+      <c r="G26" s="19">
         <v>3</v>
       </c>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="20"/>
+      <c r="T26" s="20"/>
+      <c r="U26" s="20"/>
+      <c r="V26" s="20"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="20"/>
+      <c r="Z26" s="20"/>
+      <c r="AA26" s="20"/>
+      <c r="AB26" s="18"/>
+      <c r="AC26" s="18"/>
+      <c r="AD26" s="18"/>
+      <c r="AE26" s="18"/>
+      <c r="AF26" s="18"/>
+      <c r="AG26" s="18"/>
+      <c r="AH26" s="18"/>
+      <c r="AI26" s="18"/>
+      <c r="AJ26" s="18"/>
+      <c r="AK26" s="18"/>
+      <c r="AL26" s="18"/>
+      <c r="AM26" s="18"/>
+      <c r="AN26" s="18"/>
+      <c r="AO26" s="18"/>
+      <c r="AP26" s="18"/>
+      <c r="AQ26" s="18"/>
+      <c r="AR26" s="18"/>
+      <c r="AS26" s="18"/>
+      <c r="AT26" s="18"/>
+      <c r="AU26" s="18"/>
+      <c r="AV26" s="18"/>
+      <c r="AW26" s="18"/>
+      <c r="AX26" s="18"/>
+      <c r="AY26" s="18"/>
+      <c r="AZ26" s="18"/>
+      <c r="BA26" s="18"/>
+      <c r="BB26" s="18"/>
+      <c r="BC26" s="18"/>
+      <c r="BD26" s="18"/>
+      <c r="BE26" s="18"/>
+      <c r="BF26" s="18"/>
+      <c r="BG26" s="18"/>
+      <c r="BH26" s="18"/>
+      <c r="BI26" s="18"/>
+      <c r="BJ26" s="18"/>
+      <c r="BK26" s="18"/>
+      <c r="BL26" s="18"/>
+      <c r="BM26" s="18"/>
+      <c r="BN26" s="18"/>
+      <c r="BO26" s="18"/>
+      <c r="BP26" s="18"/>
+      <c r="BQ26" s="18"/>
+      <c r="BR26" s="18"/>
+      <c r="BS26" s="18"/>
+      <c r="BT26" s="18"/>
+      <c r="BU26" s="18"/>
+      <c r="BV26" s="18"/>
+      <c r="BW26" s="18"/>
+      <c r="BX26" s="18"/>
+      <c r="BY26" s="18"/>
+      <c r="BZ26" s="18"/>
+      <c r="CA26" s="18"/>
+      <c r="CB26" s="18"/>
+      <c r="CC26" s="18"/>
+      <c r="CD26" s="18"/>
+      <c r="CE26" s="18"/>
+      <c r="CF26" s="18"/>
+      <c r="CG26" s="18"/>
     </row>
     <row r="27" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="42"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E27" s="16">
         <v>15</v>
       </c>
       <c r="F27" s="17">
+        <v>44139</v>
+      </c>
+      <c r="G27" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="29"/>
+      <c r="C28" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="16">
+        <v>15</v>
+      </c>
+      <c r="F28" s="17">
+        <v>44140</v>
+      </c>
+      <c r="G28" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="29"/>
+      <c r="C29" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="16">
+        <v>5</v>
+      </c>
+      <c r="F29" s="17">
+        <v>44141</v>
+      </c>
+      <c r="G29" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:85" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="29"/>
+      <c r="C30" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="16">
+        <v>15</v>
+      </c>
+      <c r="F30" s="17">
         <v>44142</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G30" s="4">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B14"/>
-    <mergeCell ref="B15:B22"/>
-    <mergeCell ref="B23:B27"/>
     <mergeCell ref="AK2:AR2"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:C4"/>
@@ -4145,221 +4514,117 @@
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B17"/>
+    <mergeCell ref="B18:B25"/>
+    <mergeCell ref="B26:B30"/>
   </mergeCells>
-  <conditionalFormatting sqref="H15:CG20 H22:CG25 H27:CG27 AD5:CG6 AE7:CG7 AG8:CG8 AR9:CG9 AH10:CG11 AR12:CG12 AH13:CG13 H7:AC14 AK14:CG14">
-    <cfRule type="expression" dxfId="102" priority="278">
+  <conditionalFormatting sqref="H18:CG23 H25:CG28 H30:CG30 H7:AC17 AD5:CG17">
+    <cfRule type="expression" dxfId="29" priority="374">
       <formula>KészültségiSzint</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="280">
+    <cfRule type="expression" dxfId="28" priority="376">
       <formula>KészültségiSzintTervenFelül</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="281">
+    <cfRule type="expression" dxfId="27" priority="377">
       <formula>Tényleges</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="282">
+    <cfRule type="expression" dxfId="26" priority="378">
       <formula>TénylegTervenFelül</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="283">
+    <cfRule type="expression" dxfId="25" priority="379">
       <formula>Terv</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="284">
+    <cfRule type="expression" dxfId="24" priority="380">
       <formula>H$4=időszak_kiválasztva</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="288">
+    <cfRule type="expression" dxfId="23" priority="384">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="289">
+    <cfRule type="expression" dxfId="22" priority="385">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:CG4">
-    <cfRule type="expression" dxfId="94" priority="285">
-      <formula>H$4=időszak_kiválasztva</formula>
+  <conditionalFormatting sqref="H4:CG4 F7:F17">
+    <cfRule type="expression" dxfId="21" priority="381">
+      <formula>F$4=időszak_kiválasztva</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="93" priority="77">
+    <cfRule type="expression" dxfId="20" priority="173">
       <formula>F$4=időszak_kiválasztva</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="92" priority="76">
+    <cfRule type="expression" dxfId="19" priority="172">
       <formula>F$4=időszak_kiválasztva</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F14">
-    <cfRule type="expression" dxfId="91" priority="73">
+  <conditionalFormatting sqref="F18">
+    <cfRule type="expression" dxfId="18" priority="165">
       <formula>F$4=időszak_kiválasztva</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F15">
-    <cfRule type="expression" dxfId="90" priority="69">
+  <conditionalFormatting sqref="F19:F25">
+    <cfRule type="expression" dxfId="17" priority="164">
       <formula>F$4=időszak_kiválasztva</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F16:F22">
-    <cfRule type="expression" dxfId="89" priority="68">
+  <conditionalFormatting sqref="F26:F30">
+    <cfRule type="expression" dxfId="16" priority="160">
       <formula>F$4=időszak_kiválasztva</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F23:F27">
-    <cfRule type="expression" dxfId="88" priority="64">
-      <formula>F$4=időszak_kiválasztva</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21:CG21">
-    <cfRule type="expression" dxfId="87" priority="51">
+  <conditionalFormatting sqref="H24:CG24">
+    <cfRule type="expression" dxfId="15" priority="147">
       <formula>KészültségiSzint</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="52">
+    <cfRule type="expression" dxfId="14" priority="148">
       <formula>KészültségiSzintTervenFelül</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="53">
+    <cfRule type="expression" dxfId="13" priority="149">
       <formula>Tényleges</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="54">
+    <cfRule type="expression" dxfId="12" priority="150">
       <formula>TénylegTervenFelül</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="55">
+    <cfRule type="expression" dxfId="11" priority="151">
       <formula>Terv</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="56">
+    <cfRule type="expression" dxfId="10" priority="152">
       <formula>H$4=időszak_kiválasztva</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="57">
+    <cfRule type="expression" dxfId="9" priority="153">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="58">
+    <cfRule type="expression" dxfId="8" priority="154">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H26:CG26">
-    <cfRule type="expression" dxfId="79" priority="41">
+  <conditionalFormatting sqref="H29:CG29">
+    <cfRule type="expression" dxfId="7" priority="137">
       <formula>KészültségiSzint</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="42">
+    <cfRule type="expression" dxfId="6" priority="138">
       <formula>KészültségiSzintTervenFelül</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="43">
+    <cfRule type="expression" dxfId="5" priority="139">
       <formula>Tényleges</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="44">
+    <cfRule type="expression" dxfId="4" priority="140">
       <formula>TénylegTervenFelül</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="45">
+    <cfRule type="expression" dxfId="3" priority="141">
       <formula>Terv</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="46">
+    <cfRule type="expression" dxfId="2" priority="142">
       <formula>H$4=időszak_kiválasztva</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="47">
+    <cfRule type="expression" dxfId="1" priority="143">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="48">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD9:AG9">
-    <cfRule type="expression" dxfId="71" priority="33">
-      <formula>KészültségiSzint</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="70" priority="34">
-      <formula>KészültségiSzintTervenFelül</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="69" priority="35">
-      <formula>Tényleges</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="68" priority="36">
-      <formula>TénylegTervenFelül</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="67" priority="37">
-      <formula>Terv</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="38">
-      <formula>AD$4=időszak_kiválasztva</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="39">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="40">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD11">
-    <cfRule type="expression" dxfId="63" priority="25">
-      <formula>KészültségiSzint</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="26">
-      <formula>KészültségiSzintTervenFelül</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="27">
-      <formula>Tényleges</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="28">
-      <formula>TénylegTervenFelül</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="29">
-      <formula>Terv</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="30">
-      <formula>AD$4=időszak_kiválasztva</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="31">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="32">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD12:AE12 AO12:AQ12">
-    <cfRule type="expression" dxfId="47" priority="17">
-      <formula>KészültségiSzint</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="18">
-      <formula>KészültségiSzintTervenFelül</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="19">
-      <formula>Tényleges</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="20">
-      <formula>TénylegTervenFelül</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="21">
-      <formula>Terv</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="22">
-      <formula>AD$4=időszak_kiválasztva</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="23">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="24">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD14">
-    <cfRule type="expression" dxfId="31" priority="9">
-      <formula>KészültségiSzint</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="10">
-      <formula>KészültségiSzintTervenFelül</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="11">
-      <formula>Tényleges</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="12">
-      <formula>TénylegTervenFelül</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="13">
-      <formula>Terv</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="14">
-      <formula>AD$4=időszak_kiválasztva</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="15">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="16">
+    <cfRule type="expression" dxfId="0" priority="144">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4367,7 +4632,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A projekttervező időszakokat használ az időintervallumokhoz. A kezdés=1 az 1. időszakot, az időtartam=5 pedig azt jelenti, hogy a projekt a kezdőidőszaktól számítva 5 időszakon ível át. A diagram frissítéséhez kezdjen el adatokat beírni a B5 cellától." sqref="A1:B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ez a jelmagyarázatot tartalmazó cella a terv időtartamát jelöli." sqref="J2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ez a jelmagyarázatot tartalmazó cella a projekt készültségi szintjét mutatja" sqref="W2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ez a jelmagyarázatot tartalmazó cella a tényleges időtartamot jelöli a tervezetten túl" sqref="AA2 H5:AC6 AH9:AQ9 AE8:AF8 AD13:AG13 AE11:AG11 AF12:AN12 AD7:AD8 AD10:AG10 AE14:AJ14"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ez a jelmagyarázatot tartalmazó cella a tényleges időtartamot jelöli a tervezetten túl" sqref="AA2 H5:AC6"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ez a jelmagyarázatot tartalmazó cella a projekt készültségi szintjét mutatja a tervezetten túl." sqref="AJ2"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Az időszakok 1-től 60-ig terjednek a H4-BO4 cellatartományban. " sqref="H3"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A tevékenységet a B oszlopban, a B5 cellától kezdve adhatja meg." sqref="B3:C4"/>

</xml_diff>